<commit_message>
formatted ToDo list and added env.yml file
</commit_message>
<xml_diff>
--- a/Config/config.xlsx
+++ b/Config/config.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\coswald\Desktop\GitHub Repos\missile-intercepts\Config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\coswald\Desktop\GitHub Repos\missile-intercepts\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB17C98D-02D2-4201-A7FB-E4984B1818BB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1574841A-C1AF-492F-A6D6-D65AC88292F9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{7C927F14-1512-4476-AEF4-3D0269B8EA5A}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="44">
   <si>
     <t>LP_lat_deg</t>
   </si>
@@ -141,16 +141,22 @@
     <t>missile3</t>
   </si>
   <si>
-    <t>group2</t>
-  </si>
-  <si>
-    <t>group1</t>
-  </si>
-  <si>
     <t>../Blender</t>
   </si>
   <si>
     <t>directory containing  3D COLLADA model</t>
+  </si>
+  <si>
+    <t>test_group1</t>
+  </si>
+  <si>
+    <t>test_group2</t>
+  </si>
+  <si>
+    <t>missile4</t>
+  </si>
+  <si>
+    <t>missile5</t>
   </si>
 </sst>
 </file>
@@ -608,7 +614,7 @@
   <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -687,8 +693,12 @@
       <c r="F2" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
+      <c r="G2" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>43</v>
+      </c>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
@@ -704,16 +714,20 @@
         <v>5</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
+        <v>41</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>41</v>
+      </c>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
@@ -739,8 +753,12 @@
       <c r="F4" s="6">
         <v>44042</v>
       </c>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
+      <c r="G4" s="6">
+        <v>44042</v>
+      </c>
+      <c r="H4" s="6">
+        <v>44042</v>
+      </c>
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
       <c r="K4" s="6"/>
@@ -761,13 +779,17 @@
         <v>0.16666666666666666</v>
       </c>
       <c r="E5" s="7">
-        <v>0.16666666666666666</v>
+        <v>0.16701388888888891</v>
       </c>
       <c r="F5" s="7">
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
+        <v>0.16718750000000002</v>
+      </c>
+      <c r="G5" s="7">
+        <v>0.16770833333333335</v>
+      </c>
+      <c r="H5" s="7">
+        <v>0.16805555555555554</v>
+      </c>
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
       <c r="K5" s="7"/>
@@ -785,16 +807,20 @@
         <v>6</v>
       </c>
       <c r="D6" s="13">
-        <v>39.739199999999997</v>
+        <v>39.516824999999997</v>
       </c>
       <c r="E6" s="13">
-        <v>39.757199999999997</v>
+        <v>39.485511000000002</v>
       </c>
       <c r="F6" s="13">
-        <v>39.683399999999999</v>
-      </c>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
+        <v>39.504075999999998</v>
+      </c>
+      <c r="G6" s="8">
+        <v>39.542740999999999</v>
+      </c>
+      <c r="H6" s="8">
+        <v>39.521768999999999</v>
+      </c>
       <c r="I6" s="8"/>
       <c r="J6" s="8"/>
       <c r="K6" s="8"/>
@@ -812,16 +838,20 @@
         <v>6</v>
       </c>
       <c r="D7" s="13">
-        <v>-104.97839999999999</v>
+        <v>-104.95567</v>
       </c>
       <c r="E7" s="13">
-        <v>-104.96339999999999</v>
+        <v>-104.884624</v>
       </c>
       <c r="F7" s="13">
-        <v>-105.0124</v>
-      </c>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
+        <v>-104.90361900000001</v>
+      </c>
+      <c r="G7" s="8">
+        <v>-104.97689699999999</v>
+      </c>
+      <c r="H7" s="8">
+        <v>-105.01303799999999</v>
+      </c>
       <c r="I7" s="8"/>
       <c r="J7" s="8"/>
       <c r="K7" s="8"/>
@@ -839,16 +869,20 @@
         <v>6</v>
       </c>
       <c r="D8" s="13">
-        <v>41.14</v>
+        <v>40.862397000000001</v>
       </c>
       <c r="E8" s="13">
-        <v>41.14</v>
+        <v>40.862397000000001</v>
       </c>
       <c r="F8" s="13">
-        <v>41.14</v>
-      </c>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
+        <v>40.862397000000001</v>
+      </c>
+      <c r="G8" s="13">
+        <v>40.862397000000001</v>
+      </c>
+      <c r="H8" s="13">
+        <v>40.862397000000001</v>
+      </c>
       <c r="I8" s="8"/>
       <c r="J8" s="8"/>
       <c r="K8" s="8"/>
@@ -866,16 +900,20 @@
         <v>6</v>
       </c>
       <c r="D9" s="13">
-        <v>-104.8202</v>
+        <v>-105.025902</v>
       </c>
       <c r="E9" s="13">
-        <v>-104.8202</v>
+        <v>-105.025902</v>
       </c>
       <c r="F9" s="13">
-        <v>-104.8202</v>
-      </c>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
+        <v>-105.025902</v>
+      </c>
+      <c r="G9" s="13">
+        <v>-105.025902</v>
+      </c>
+      <c r="H9" s="13">
+        <v>-105.025902</v>
+      </c>
       <c r="I9" s="8"/>
       <c r="J9" s="8"/>
       <c r="K9" s="8"/>
@@ -901,8 +939,12 @@
       <c r="F10" s="9">
         <v>1</v>
       </c>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
+      <c r="G10" s="9">
+        <v>1</v>
+      </c>
+      <c r="H10" s="9">
+        <v>1</v>
+      </c>
       <c r="I10" s="9"/>
       <c r="J10" s="9"/>
       <c r="K10" s="9"/>
@@ -928,8 +970,12 @@
       <c r="F11" s="9">
         <v>1</v>
       </c>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
+      <c r="G11" s="9">
+        <v>1</v>
+      </c>
+      <c r="H11" s="9">
+        <v>1</v>
+      </c>
       <c r="I11" s="9"/>
       <c r="J11" s="9"/>
       <c r="K11" s="9"/>
@@ -955,8 +1001,12 @@
       <c r="F12" s="9">
         <v>10</v>
       </c>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
+      <c r="G12" s="9">
+        <v>10</v>
+      </c>
+      <c r="H12" s="9">
+        <v>10</v>
+      </c>
       <c r="I12" s="9"/>
       <c r="J12" s="9"/>
       <c r="K12" s="9"/>
@@ -982,8 +1032,12 @@
       <c r="F13" s="9">
         <v>10</v>
       </c>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
+      <c r="G13" s="9">
+        <v>10</v>
+      </c>
+      <c r="H13" s="9">
+        <v>10</v>
+      </c>
       <c r="I13" s="9"/>
       <c r="J13" s="9"/>
       <c r="K13" s="9"/>
@@ -995,22 +1049,26 @@
         <v>15</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
+        <v>38</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>38</v>
+      </c>
       <c r="I14" s="9"/>
       <c r="J14" s="9"/>
       <c r="K14" s="9"/>
@@ -1036,8 +1094,12 @@
       <c r="F15" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
+      <c r="G15" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H15" s="9" t="s">
+        <v>17</v>
+      </c>
       <c r="I15" s="9"/>
       <c r="J15" s="9"/>
       <c r="K15" s="9"/>
@@ -1063,8 +1125,12 @@
       <c r="F16" s="11">
         <v>500</v>
       </c>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
+      <c r="G16" s="11">
+        <v>500</v>
+      </c>
+      <c r="H16" s="11">
+        <v>500</v>
+      </c>
       <c r="I16" s="11"/>
       <c r="J16" s="11"/>
       <c r="K16" s="11"/>

</xml_diff>